<commit_message>
Update xlsx format for batch proccesor
</commit_message>
<xml_diff>
--- a/translate_files.xlsx
+++ b/translate_files.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>INPUT_FILE_PATH_FOLDER</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>E:\Debby\9_Scripts\TranslateHTML\Translate_HTML_XML_v11\database\PDR_enu_esp_database.json</t>
+  </si>
+  <si>
+    <t>REGION_TABLE_PATH</t>
+  </si>
+  <si>
+    <t>REFER_TEXT_TABLE_PATH</t>
   </si>
 </sst>
 </file>
@@ -402,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,12 +424,12 @@
     <col min="6" max="6" width="12.140625" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="9" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -452,16 +458,22 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -486,10 +498,10 @@
       <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="b">
+      <c r="L2" t="b">
         <v>0</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>